<commit_message>
Create sankey from existing budget fond files
</commit_message>
<xml_diff>
--- a/public/files/fond_revenues.xlsx
+++ b/public/files/fond_revenues.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
@@ -112,7 +112,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -125,9 +125,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -165,7 +165,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -237,7 +237,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -411,9 +411,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:C92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79:C92"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1013,7 +1015,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>24110900</v>
       </c>
@@ -1022,7 +1024,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>24170000</v>
       </c>
@@ -1031,7 +1033,7 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>25000000</v>
       </c>
@@ -1040,7 +1042,7 @@
         <v>16784600</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>25010000</v>
       </c>
@@ -1049,7 +1051,7 @@
         <v>16784600</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>25010100</v>
       </c>
@@ -1058,7 +1060,7 @@
         <v>16784600</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>30000000</v>
       </c>
@@ -1067,7 +1069,7 @@
         <v>19605130</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>31000000</v>
       </c>
@@ -1076,7 +1078,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>31030000</v>
       </c>
@@ -1085,7 +1087,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>33000000</v>
       </c>
@@ -1094,7 +1096,7 @@
         <v>11605130</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>33010000</v>
       </c>
@@ -1103,7 +1105,7 @@
         <v>11605130</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>33010100</v>
       </c>
@@ -1112,7 +1114,7 @@
         <v>9928800</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>33010400</v>
       </c>
@@ -1121,7 +1123,7 @@
         <v>1676330</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>50000000</v>
       </c>
@@ -1130,7 +1132,7 @@
         <v>895300</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>50110000</v>
       </c>
@@ -1139,139 +1141,139 @@
         <v>895300</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="1">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
         <v>40000000</v>
       </c>
+      <c r="B79" s="2">
+        <v>401833900</v>
+      </c>
+      <c r="C79" s="2">
+        <v>12872700</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>41000000</v>
+      </c>
+      <c r="B80" s="2">
+        <v>401833900</v>
+      </c>
       <c r="C80" s="2">
-        <v>401833900</v>
-      </c>
-      <c r="D80" s="2">
         <v>12872700</v>
       </c>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="1">
-        <v>41000000</v>
-      </c>
-      <c r="C81" s="2">
-        <v>401833900</v>
-      </c>
-      <c r="D81" s="2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>41020000</v>
+      </c>
+      <c r="B81" s="2">
+        <v>102022400</v>
+      </c>
+      <c r="C81" s="3"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>41020100</v>
+      </c>
+      <c r="B82" s="2">
+        <v>102022400</v>
+      </c>
+      <c r="C82" s="3"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>41030000</v>
+      </c>
+      <c r="B83" s="2">
+        <v>299811500</v>
+      </c>
+      <c r="C83" s="2">
         <v>12872700</v>
       </c>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="1">
-        <v>41020000</v>
-      </c>
-      <c r="C82" s="2">
-        <v>102022400</v>
-      </c>
-      <c r="D82" s="3"/>
-    </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="1">
-        <v>41020100</v>
-      </c>
-      <c r="C83" s="2">
-        <v>102022400</v>
-      </c>
-      <c r="D83" s="3"/>
-    </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="1">
-        <v>41030000</v>
-      </c>
-      <c r="C84" s="2">
-        <v>299811500</v>
-      </c>
-      <c r="D84" s="2">
-        <v>12872700</v>
-      </c>
-    </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="1">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
         <v>41030601</v>
       </c>
-      <c r="C85" s="2">
+      <c r="B84" s="2">
         <v>246745700</v>
       </c>
-      <c r="D85" s="3"/>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="1">
+      <c r="C84" s="3"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
         <v>41030801</v>
       </c>
-      <c r="C86" s="2">
+      <c r="B85" s="2">
         <v>28371200</v>
       </c>
-      <c r="D86" s="3"/>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="1">
+      <c r="C85" s="3"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
         <v>41030901</v>
       </c>
-      <c r="C87" s="2">
+      <c r="B86" s="2">
         <v>17661000</v>
       </c>
-      <c r="D87" s="3"/>
-    </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="1">
+      <c r="C86" s="3"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
         <v>41031001</v>
       </c>
-      <c r="C88" s="4">
+      <c r="B87" s="4">
         <v>700</v>
       </c>
-      <c r="D88" s="3"/>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="1">
+      <c r="C87" s="3"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
         <v>41034400</v>
       </c>
+      <c r="B88" s="3"/>
+      <c r="C88" s="2">
+        <v>12364000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>41034800</v>
+      </c>
+      <c r="B89" s="2">
+        <v>936300</v>
+      </c>
       <c r="C89" s="3"/>
-      <c r="D89" s="2">
-        <v>12364000</v>
-      </c>
-    </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="1">
-        <v>41034800</v>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>41035000</v>
+      </c>
+      <c r="B90" s="2">
+        <v>5171900</v>
       </c>
       <c r="C90" s="2">
-        <v>936300</v>
-      </c>
-      <c r="D90" s="3"/>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="1">
-        <v>41035000</v>
-      </c>
-      <c r="C91" s="2">
-        <v>5171900</v>
-      </c>
-      <c r="D91" s="2">
         <v>508700</v>
       </c>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="1">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
         <v>41035800</v>
       </c>
-      <c r="C92" s="2">
+      <c r="B91" s="2">
         <v>609700</v>
       </c>
-      <c r="D92" s="3"/>
-    </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B93" s="1">
+      <c r="C91" s="3"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
         <v>41036300</v>
       </c>
-      <c r="C93" s="2">
+      <c r="B92" s="2">
         <v>315000</v>
       </c>
-      <c r="D93" s="3"/>
+      <c r="C92" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>